<commit_message>
Updated July deterministic comparison using new ruleset
added new ruleset to July folder (ruleset used for most recent testing)
Reran the MRM, new output files and model files for each trace included in the push
</commit_message>
<xml_diff>
--- a/RW Files/TestModelRuns/07_July Models/MtomToCrss_Annual.xlsx
+++ b/RW Files/TestModelRuns/07_July Models/MtomToCrss_Annual.xlsx
@@ -2123,13 +2123,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>10069807.747840716</v>
+        <v>10069807.79058357</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>10352228.051840715</v>
+        <v>10352228.094583571</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -3329,13 +3329,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8587570.2131973114</v>
+        <v>8587570.2347199731</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8728198.2431973144</v>
+        <v>8728198.2647199742</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -7952,13 +7952,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8617022.5327112917</v>
+        <v>8617022.5542262942</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8767620.2027112935</v>
+        <v>8767620.2242262959</v>
       </c>
       <c r="U3">
         <v>0</v>

</xml_diff>